<commit_message>
Completed funds and income functions
</commit_message>
<xml_diff>
--- a/output/Expenditure.xlsx
+++ b/output/Expenditure.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,24 +539,145 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Gpay</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="n"/>
+      <c r="I4" s="4" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n"/>
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="n"/>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>1700</v>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Gpay</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="n"/>
+      <c r="I5" s="4" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n"/>
+      <c r="F6" s="3" t="n"/>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="n"/>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>400</v>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Card</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="n"/>
+      <c r="I7" s="4" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="n"/>
+      <c r="E8" s="3" t="n"/>
+      <c r="F8" s="3" t="n"/>
+      <c r="G8" s="3" t="n"/>
+      <c r="H8" s="4" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n"/>
-      <c r="C4" s="2">
-        <f>SUM(C3:C3)</f>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2">
+        <f>SUM(C3:C8)</f>
         <v/>
       </c>
-      <c r="D4" s="2" t="n"/>
-      <c r="E4" s="3" t="n"/>
-      <c r="F4" s="3">
-        <f>SUM(F3:F3)</f>
+      <c r="D9" s="2" t="n"/>
+      <c r="E9" s="3" t="n"/>
+      <c r="F9" s="3">
+        <f>SUM(F3:F8)</f>
         <v/>
       </c>
-      <c r="G4" s="3" t="n"/>
-      <c r="H4" s="4" t="n"/>
-      <c r="I4" s="4">
-        <f>SUM(I3:I3)</f>
+      <c r="G9" s="3" t="n"/>
+      <c r="H9" s="4" t="n"/>
+      <c r="I9" s="4">
+        <f>SUM(I3:I8)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a savings column in the output
</commit_message>
<xml_diff>
--- a/output/Expenditure.xlsx
+++ b/output/Expenditure.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -53,6 +53,11 @@
         <fgColor rgb="00A9D08E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFD966"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -66,7 +71,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -78,6 +83,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -445,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +510,7 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="J1" s="5" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
@@ -510,6 +522,7 @@
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
+      <c r="J2" s="5" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -535,6 +548,7 @@
       <c r="G3" s="3" t="n"/>
       <c r="H3" s="4" t="n"/>
       <c r="I3" s="4" t="n"/>
+      <c r="J3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -560,6 +574,7 @@
       </c>
       <c r="H4" s="4" t="n"/>
       <c r="I4" s="4" t="n"/>
+      <c r="J4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -585,6 +600,7 @@
       </c>
       <c r="H5" s="4" t="n"/>
       <c r="I5" s="4" t="n"/>
+      <c r="J5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -610,6 +626,7 @@
       <c r="G6" s="3" t="n"/>
       <c r="H6" s="4" t="n"/>
       <c r="I6" s="4" t="n"/>
+      <c r="J6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -635,6 +652,7 @@
       </c>
       <c r="H7" s="4" t="n"/>
       <c r="I7" s="4" t="n"/>
+      <c r="J7" s="5" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -656,28 +674,111 @@
       <c r="I8" s="4" t="n">
         <v>15000</v>
       </c>
+      <c r="J8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n"/>
-      <c r="C9" s="2">
-        <f>SUM(C3:C8)</f>
-        <v/>
-      </c>
-      <c r="D9" s="2" t="n"/>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Gpay</t>
+        </is>
+      </c>
       <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3">
-        <f>SUM(F3:F8)</f>
-        <v/>
-      </c>
+      <c r="F9" s="3" t="n"/>
       <c r="G9" s="3" t="n"/>
       <c r="H9" s="4" t="n"/>
-      <c r="I9" s="4">
-        <f>SUM(I3:I8)</f>
+      <c r="I9" s="4" t="n"/>
+      <c r="J9" s="6" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Cab</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>444</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Gpay</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="n"/>
+      <c r="F10" s="3" t="n"/>
+      <c r="G10" s="3" t="n"/>
+      <c r="H10" s="4" t="n"/>
+      <c r="I10" s="4" t="n"/>
+      <c r="J10" s="6" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>31-8-2022</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Cab</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>444</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Gpay</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n"/>
+      <c r="F11" s="3" t="n"/>
+      <c r="G11" s="3" t="n"/>
+      <c r="H11" s="4" t="n"/>
+      <c r="I11" s="4" t="n"/>
+      <c r="J11" s="6" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2">
+        <f>SUM(C3:C11)</f>
+        <v/>
+      </c>
+      <c r="D12" s="2" t="n"/>
+      <c r="E12" s="3" t="n"/>
+      <c r="F12" s="3">
+        <f>SUM(F3:F11)</f>
+        <v/>
+      </c>
+      <c r="G12" s="3" t="n"/>
+      <c r="H12" s="4" t="n"/>
+      <c r="I12" s="4">
+        <f>SUM(I3:I11)</f>
+        <v/>
+      </c>
+      <c r="J12" s="6">
+        <f>I12-F12-C12</f>
         <v/>
       </c>
     </row>

</xml_diff>